<commit_message>
code plus rapide par clusters
</commit_message>
<xml_diff>
--- a/data/ping.xlsx
+++ b/data/ping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phbro\Desktop\DOCUMENTS\ActuRank\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997891A6-8AEF-45C5-8B6F-A1B32E56EE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6795B38-572D-4A68-B028-9A5FB7C8F838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="768" windowWidth="16440" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3160" uniqueCount="106">
   <si>
     <t>players</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>19/09/2024</t>
+  </si>
+  <si>
+    <t>26/09/2024</t>
   </si>
 </sst>
 </file>
@@ -742,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O996"/>
+  <dimension ref="A1:O1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A970" workbookViewId="0">
-      <selection activeCell="J993" sqref="J993"/>
+    <sheetView tabSelected="1" topLeftCell="A994" workbookViewId="0">
+      <selection activeCell="G1008" sqref="G1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32020,7 +32023,7 @@
         <v>96</v>
       </c>
       <c r="K939" s="10" t="str">
-        <f t="shared" ref="K939:K996" si="27">IF(OR(OR(AND(OR(A939=B939,A939=C939,A939=D939,B939=C939,B939=D939,C939=D939),OR(A939&lt;&gt;"",D939&lt;&gt;"")),H939&gt;MAX(F939:G939),B939=C939),OR(AND(ISBLANK(A939)=FALSE,ISNA(VLOOKUP(A939,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B939,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C939,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D939)=FALSE,ISNA(VLOOKUP(D939,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A939:D939)=1,COUNTBLANK(A939:D939)=3))),"ERREUR","")</f>
+        <f t="shared" ref="K939:K1008" si="27">IF(OR(OR(AND(OR(A939=B939,A939=C939,A939=D939,B939=C939,B939=D939,C939=D939),OR(A939&lt;&gt;"",D939&lt;&gt;"")),H939&gt;MAX(F939:G939),B939=C939),OR(AND(ISBLANK(A939)=FALSE,ISNA(VLOOKUP(A939,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B939,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C939,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D939)=FALSE,ISNA(VLOOKUP(D939,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A939:D939)=1,COUNTBLANK(A939:D939)=3))),"ERREUR","")</f>
         <v/>
       </c>
     </row>
@@ -32060,7 +32063,7 @@
         <v>14</v>
       </c>
       <c r="E941" s="1">
-        <f t="shared" ref="E941:E996" si="28">IF(F941&gt;G941,1,0)</f>
+        <f t="shared" ref="E941:E1008" si="28">IF(F941&gt;G941,1,0)</f>
         <v>1</v>
       </c>
       <c r="F941" s="5">
@@ -33616,6 +33619,342 @@
         <v>104</v>
       </c>
       <c r="K996" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="997" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B997" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C997" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E997" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F997" s="5">
+        <v>7</v>
+      </c>
+      <c r="G997" s="5">
+        <v>5</v>
+      </c>
+      <c r="H997" s="1">
+        <v>7</v>
+      </c>
+      <c r="I997" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K997" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="998" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B998" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C998" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E998" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F998" s="5">
+        <v>7</v>
+      </c>
+      <c r="G998" s="5">
+        <v>4</v>
+      </c>
+      <c r="H998" s="1">
+        <v>7</v>
+      </c>
+      <c r="I998" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K998" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="999" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B999" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C999" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E999" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F999" s="5">
+        <v>8</v>
+      </c>
+      <c r="G999" s="5">
+        <v>6</v>
+      </c>
+      <c r="H999" s="1">
+        <v>7</v>
+      </c>
+      <c r="I999" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K999" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1000" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1000" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1000" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1000" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1000" s="5">
+        <v>8</v>
+      </c>
+      <c r="G1000" s="5">
+        <v>6</v>
+      </c>
+      <c r="H1000" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1000" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1000" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1001" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1001" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1001" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1001" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1001" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1001" s="5">
+        <v>4</v>
+      </c>
+      <c r="H1001" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1001" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1001" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1002" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1002" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1002" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1002" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1002" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1002" s="5">
+        <v>5</v>
+      </c>
+      <c r="H1002" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1002" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1002" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1003" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1003" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1003" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1003" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1003" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1003" s="5">
+        <v>1</v>
+      </c>
+      <c r="H1003" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1003" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1003" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1004" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1004" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1004" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1004" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1004" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1004" s="5">
+        <v>3</v>
+      </c>
+      <c r="H1004" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1004" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1004" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1005" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1005" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1005" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1005" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1005" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1005" s="5">
+        <v>4</v>
+      </c>
+      <c r="H1005" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1005" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1005" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1006" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1006" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1006" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1006" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1006" s="5">
+        <v>9</v>
+      </c>
+      <c r="G1006" s="5">
+        <v>7</v>
+      </c>
+      <c r="H1006" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1006" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1006" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1007" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1007" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1007" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1007" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1007" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1007" s="5">
+        <v>4</v>
+      </c>
+      <c r="H1007" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1007" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1007" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="1008" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1008" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1008" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1008" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F1008" s="5">
+        <v>7</v>
+      </c>
+      <c r="G1008" s="5">
+        <v>2</v>
+      </c>
+      <c r="H1008" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1008" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1008" s="10" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>

</xml_diff>